<commit_message>
atualização do dashboard de vendas do Xbox com Excel
</commit_message>
<xml_diff>
--- a/DASHBOARD DE VENDAS DO XBOX COM EXCEL.xlsx
+++ b/DASHBOARD DE VENDAS DO XBOX COM EXCEL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/afd79c59625de37d/PROJETOS/DASHBOARD DE VENDAS DO XBOX COM EXCEL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_A7AE2295331C573B2CB46D73BF63A0ABC8B04942" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC52DB8F-6DA2-49A4-AF48-F50DB9D23109}"/>
+  <xr:revisionPtr revIDLastSave="180" documentId="11_A7AE2295331C573B2CB46D73BF63A0ABC8B04942" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ECF6A4B7-1669-4800-BC03-42F7373CC8E9}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2008" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2017" uniqueCount="320">
   <si>
     <t>Paleta de Cores</t>
   </si>
@@ -1090,14 +1090,21 @@
   <si>
     <t>Soma de EA Play Season Pass</t>
   </si>
+  <si>
+    <t>Pergunta Negócio 4 - Total de Vendas de Assinaturas do Minecraft Season Pass.</t>
+  </si>
+  <si>
+    <t>Soma de Minecraft Season Pass Price</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00;[Red]&quot;R$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="170" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -1237,7 +1244,7 @@
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1269,6 +1276,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Moeda" xfId="2" builtinId="4"/>
@@ -1276,7 +1285,29 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Título 1" xfId="1" builtinId="16"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+        <name val="Aptos Black"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0F7C10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0F7C10"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1342,12 +1373,16 @@
       </border>
     </dxf>
   </dxfs>
-  <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+  <tableStyles count="3" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Estilo de Segmentação de Dados 1" pivot="0" table="0" count="5" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="15"/>
-      <tableStyleElement type="headerRow" dxfId="14"/>
+      <tableStyleElement type="wholeTable" dxfId="17"/>
+      <tableStyleElement type="headerRow" dxfId="16"/>
     </tableStyle>
     <tableStyle name="Estilo de Segmentação de Dados 2" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}"/>
+    <tableStyle name="Estilo de Segmentação de Dados 3" pivot="0" table="0" count="10" xr9:uid="{0ECB9299-9BC6-4CDF-AB1E-90EE5F283DC8}">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
   </tableStyles>
   <colors>
     <mruColors>
@@ -1365,7 +1400,63 @@
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{46F421CA-312F-682f-3DD2-61675219B42D}">
-      <x14:dxfs count="5">
+      <x14:dxfs count="13">
+        <dxf>
+          <fill>
+            <patternFill>
+              <bgColor theme="9" tint="-0.24994659260841701"/>
+            </patternFill>
+          </fill>
+        </dxf>
+        <dxf>
+          <fill>
+            <patternFill>
+              <bgColor theme="9" tint="-0.24994659260841701"/>
+            </patternFill>
+          </fill>
+        </dxf>
+        <dxf>
+          <fill>
+            <patternFill>
+              <bgColor theme="9" tint="-0.24994659260841701"/>
+            </patternFill>
+          </fill>
+        </dxf>
+        <dxf>
+          <fill>
+            <patternFill>
+              <bgColor theme="9" tint="-0.24994659260841701"/>
+            </patternFill>
+          </fill>
+        </dxf>
+        <dxf>
+          <fill>
+            <patternFill>
+              <bgColor rgb="FFC00000"/>
+            </patternFill>
+          </fill>
+        </dxf>
+        <dxf>
+          <fill>
+            <patternFill>
+              <bgColor theme="9" tint="0.39994506668294322"/>
+            </patternFill>
+          </fill>
+        </dxf>
+        <dxf>
+          <fill>
+            <patternFill>
+              <bgColor theme="9" tint="-0.24994659260841701"/>
+            </patternFill>
+          </fill>
+        </dxf>
+        <dxf>
+          <fill>
+            <patternFill>
+              <bgColor theme="0"/>
+            </patternFill>
+          </fill>
+        </dxf>
         <dxf>
           <border>
             <horizontal style="thin">
@@ -1417,15 +1508,27 @@
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1">
         <x14:slicerStyle name="Estilo de Segmentação de Dados 1">
           <x14:slicerStyleElements>
-            <x14:slicerStyleElement type="selectedItemWithData" dxfId="4"/>
-            <x14:slicerStyleElement type="selectedItemWithNoData" dxfId="3"/>
-            <x14:slicerStyleElement type="hoveredSelectedItemWithNoData" dxfId="2"/>
+            <x14:slicerStyleElement type="selectedItemWithData" dxfId="12"/>
+            <x14:slicerStyleElement type="selectedItemWithNoData" dxfId="11"/>
+            <x14:slicerStyleElement type="hoveredSelectedItemWithNoData" dxfId="10"/>
           </x14:slicerStyleElements>
         </x14:slicerStyle>
         <x14:slicerStyle name="Estilo de Segmentação de Dados 2">
           <x14:slicerStyleElements>
-            <x14:slicerStyleElement type="selectedItemWithData" dxfId="1"/>
-            <x14:slicerStyleElement type="selectedItemWithNoData" dxfId="0"/>
+            <x14:slicerStyleElement type="selectedItemWithData" dxfId="9"/>
+            <x14:slicerStyleElement type="selectedItemWithNoData" dxfId="8"/>
+          </x14:slicerStyleElements>
+        </x14:slicerStyle>
+        <x14:slicerStyle name="Estilo de Segmentação de Dados 3">
+          <x14:slicerStyleElements>
+            <x14:slicerStyleElement type="unselectedItemWithData" dxfId="7"/>
+            <x14:slicerStyleElement type="unselectedItemWithNoData" dxfId="6"/>
+            <x14:slicerStyleElement type="selectedItemWithData" dxfId="5"/>
+            <x14:slicerStyleElement type="selectedItemWithNoData" dxfId="4"/>
+            <x14:slicerStyleElement type="hoveredUnselectedItemWithData" dxfId="3"/>
+            <x14:slicerStyleElement type="hoveredSelectedItemWithData" dxfId="2"/>
+            <x14:slicerStyleElement type="hoveredUnselectedItemWithNoData" dxfId="1"/>
+            <x14:slicerStyleElement type="hoveredSelectedItemWithNoData" dxfId="0"/>
           </x14:slicerStyleElements>
         </x14:slicerStyle>
       </x14:slicerStyles>
@@ -1487,8 +1590,9 @@
         <c:idx val="2"/>
         <c:spPr>
           <a:solidFill>
-            <a:schemeClr val="bg2">
-              <a:lumMod val="75000"/>
+            <a:schemeClr val="accent3">
+              <a:lumMod val="60000"/>
+              <a:lumOff val="40000"/>
             </a:schemeClr>
           </a:solidFill>
         </c:spPr>
@@ -1497,11 +1601,97 @@
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
-          <c:delete val="1"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="b" anchorCtr="0">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="r">
+                <a:defRPr sz="1100" b="1">
+                  <a:solidFill>
+                    <a:schemeClr val="accent6">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
           <c:extLst>
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
           </c:extLst>
         </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:layout>
+            <c:manualLayout>
+              <c:x val="-1.9372626965125303E-16"/>
+              <c:y val="-3.5991306902043199E-17"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="b" anchorCtr="0">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="r">
+                <a:defRPr sz="1100" b="1">
+                  <a:solidFill>
+                    <a:schemeClr val="accent6">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+              <c15:layout>
+                <c:manualLayout>
+                  <c:w val="9.4031417661156413E-2"/>
+                  <c:h val="6.011987980561273E-2"/>
+                </c:manualLayout>
+              </c15:layout>
+            </c:ext>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
       </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
@@ -1510,10 +1700,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.25732386825992476"/>
-          <c:y val="0.19547275340582426"/>
-          <c:w val="0.65731845892350005"/>
-          <c:h val="0.72831906097677246"/>
+          <c:x val="3.4130921835677182E-2"/>
+          <c:y val="0.11945271374218566"/>
+          <c:w val="0.95107329283432807"/>
+          <c:h val="0.81745675673518625"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -1536,12 +1726,105 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="bg2">
-                <a:lumMod val="75000"/>
+              <a:schemeClr val="accent3">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
               </a:schemeClr>
             </a:solidFill>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.9372626965125303E-16"/>
+                  <c:y val="-3.5991306902043199E-17"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="b" anchorCtr="0">
+                  <a:noAutofit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr algn="r">
+                    <a:defRPr sz="1100" b="1">
+                      <a:solidFill>
+                        <a:schemeClr val="accent6">
+                          <a:lumMod val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="pt-BR"/>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="9.4031417661156413E-2"/>
+                      <c:h val="6.011987980561273E-2"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-756E-49A0-95CB-85120648B4A6}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="b" anchorCtr="0">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="r">
+                  <a:defRPr sz="1100" b="1">
+                    <a:solidFill>
+                      <a:schemeClr val="accent6">
+                        <a:lumMod val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Cálculos!$B$12:$B$14</c:f>
@@ -1563,10 +1846,10 @@
                 <c:formatCode>"R$"\ #,##0.00;[Red]"R$"\ #,##0.00</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>2824</c:v>
+                  <c:v>217</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>747</c:v>
+                  <c:v>1537</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1612,9 +1895,8 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="b"/>
-        <c:majorGridlines/>
         <c:numFmt formatCode="&quot;R$&quot;\ #,##0.00;[Red]&quot;R$&quot;\ #,##0.00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -1639,13 +1921,12 @@
     <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId1"/>
   <c:extLst>
     <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
       <c14:pivotOptions>
         <c14:dropZoneFilter val="1"/>
         <c14:dropZoneCategories val="1"/>
-        <c14:dropZoneData val="1"/>
-        <c14:dropZonesVisible val="1"/>
       </c14:pivotOptions>
     </c:ext>
   </c:extLst>
@@ -1758,8 +2039,8 @@
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>619125</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>264192</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1789,8 +2070,57 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="723900" y="5762625"/>
-          <a:ext cx="3324225" cy="857250"/>
+          <a:off x="647700" y="6029325"/>
+          <a:ext cx="3274092" cy="904875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>95252</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>236453</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>58104</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagem 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect t="39200" b="40200"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609599" y="5200652"/>
+          <a:ext cx="3284454" cy="724852"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1807,8 +2137,8 @@
       <xdr:rowOff>104776</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>666750</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>173102</xdr:rowOff>
     </xdr:to>
@@ -1826,7 +2156,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1839,8 +2169,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="695325" y="3810001"/>
-          <a:ext cx="3400425" cy="1420876"/>
+          <a:off x="619125" y="3990976"/>
+          <a:ext cx="3305175" cy="1478026"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1851,23 +2181,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>676274</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>95252</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>58104</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>573640</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Imagem 6">
+        <xdr:cNvPr id="3" name="Imagem 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{224DA4D8-B447-AE67-11A7-09817AA944FE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1876,20 +2206,72 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect t="39200" b="40200"/>
-        <a:stretch/>
+        <a:srcRect l="63987" t="22222" r="7717" b="22840"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676274" y="4972052"/>
-          <a:ext cx="3333751" cy="686752"/>
+          <a:off x="7848600" y="4181475"/>
+          <a:ext cx="649840" cy="657225"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>62217</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>433367</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Imagem 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2560858A-A59F-F89E-23C9-270E43D714C0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6610350" y="4205592"/>
+          <a:ext cx="1138217" cy="852183"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2004,6 +2386,177 @@
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>143934</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>32809</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>349250</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>51859</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="13" name="Agrupar 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBF83B8C-85F8-3937-0A83-C59CC6A2F887}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1739372" y="2378340"/>
+          <a:ext cx="9920816" cy="3829050"/>
+          <a:chOff x="1636183" y="911225"/>
+          <a:chExt cx="4948767" cy="3829050"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="8" name="Retângulo de cantos arredondados 7">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000008000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1636183" y="911225"/>
+            <a:ext cx="4948767" cy="3829050"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 6196"/>
+            </a:avLst>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent6"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent6"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="pt-BR" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:graphicFrame macro="">
+        <xdr:nvGraphicFramePr>
+          <xdr:cNvPr id="6" name="Gráfico 5">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000006000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGraphicFramePr>
+            <a:graphicFrameLocks/>
+          </xdr:cNvGraphicFramePr>
+        </xdr:nvGraphicFramePr>
+        <xdr:xfrm>
+          <a:off x="1727446" y="1263376"/>
+          <a:ext cx="4796133" cy="3234540"/>
+        </xdr:xfrm>
+        <a:graphic>
+          <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+            <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          </a:graphicData>
+        </a:graphic>
+      </xdr:graphicFrame>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>35719</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>35719</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="Retângulo: Cantos Superiores Arredondados 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7AEF5A12-B994-92E9-CE28-9885067187B8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1738313" y="2381250"/>
+          <a:ext cx="9906000" cy="571500"/>
+        </a:xfrm>
+        <a:prstGeom prst="round2SameRect">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 43750"/>
+            <a:gd name="adj2" fmla="val 0"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="lt1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -2031,7 +2584,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2117,109 +2670,6 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="10" name="Grupo 9">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000A000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="1636183" y="911225"/>
-          <a:ext cx="4948767" cy="3829050"/>
-          <a:chOff x="1866900" y="904875"/>
-          <a:chExt cx="5524500" cy="3638550"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="8" name="Retângulo de cantos arredondados 7">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000008000000}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="1866900" y="904875"/>
-            <a:ext cx="5524500" cy="3638550"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst>
-              <a:gd name="adj" fmla="val 6196"/>
-            </a:avLst>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent6"/>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="lt1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent6"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="pt-BR" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:graphicFrame macro="">
-        <xdr:nvGraphicFramePr>
-          <xdr:cNvPr id="6" name="Gráfico 5">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000006000000}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvGraphicFramePr>
-            <a:graphicFrameLocks/>
-          </xdr:cNvGraphicFramePr>
-        </xdr:nvGraphicFramePr>
-        <xdr:xfrm>
-          <a:off x="1962150" y="990600"/>
-          <a:ext cx="5257799" cy="3333750"/>
-        </xdr:xfrm>
-        <a:graphic>
-          <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-            <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-          </a:graphicData>
-        </a:graphic>
-      </xdr:graphicFrame>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -2302,22 +2752,249 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>161924</xdr:rowOff>
+      <xdr:colOff>122767</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>98424</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>19049</xdr:rowOff>
+      <xdr:colOff>170392</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>146049</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="14" name="Agrupar 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF16270E-38F1-582F-6E36-82407AB6492E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1718205" y="919955"/>
+          <a:ext cx="4905375" cy="1381125"/>
+          <a:chOff x="1636183" y="4797424"/>
+          <a:chExt cx="4958292" cy="1381125"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="9" name="Retângulo de cantos arredondados 8">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000009000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1636183" y="4797424"/>
+            <a:ext cx="4958292" cy="1381125"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 15685"/>
+            </a:avLst>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent6"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent6"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="pt-BR" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="Cálculos!E25">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="11" name="Retângulo de cantos arredondados 10">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000B000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2907236" y="4943476"/>
+            <a:ext cx="2888191" cy="904876"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 15685"/>
+            </a:avLst>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent6">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent6"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent6"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:fld id="{52D6CB36-8EA5-4E73-BBE0-2A585CF0AFAC}" type="TxLink">
+              <a:rPr lang="pt-BR" sz="3600"/>
+              <a:pPr algn="ctr"/>
+              <a:t>R$ 600,00</a:t>
+            </a:fld>
+            <a:endParaRPr lang="pt-BR" sz="3600"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="2" name="CaixaDeTexto 1">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86503129-72BD-3343-611C-FEE3F61C6ECB}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2635244" y="5894917"/>
+            <a:ext cx="3386666" cy="243417"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="accent5"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="pt-BR" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>TOTAL SUBSCRIPTIONS EA/PEASON PASS</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-BR" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="12" name="Imagem 11">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81601C07-6AF9-4E6B-ADAD-DEF8A3DCEB71}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill rotWithShape="1">
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect l="63987" t="22222" r="7717" b="22840"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1866911" y="4956795"/>
+            <a:ext cx="916506" cy="926922"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>275167</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>92074</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>322792</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>139699</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="Retângulo de cantos arredondados 8">
+        <xdr:cNvPr id="16" name="Retângulo de cantos arredondados 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59A53AFF-C44B-ADCD-0E5D-FA9DF76CEA61}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2325,8 +3002,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1866900" y="4600574"/>
-          <a:ext cx="5534025" cy="1304925"/>
+          <a:off x="6783917" y="917574"/>
+          <a:ext cx="4958292" cy="1381125"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -2361,23 +3038,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>180974</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>551386</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>47626</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>370411</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>2</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="Cálculos!E21">
+    <xdr:sp macro="" textlink="Cálculos!E35">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="Retângulo de cantos arredondados 10">
+        <xdr:cNvPr id="17" name="Retângulo de cantos arredondados 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE46F2A9-75F9-F0A5-50DE-0C8830CDB51D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2385,8 +3062,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3019425" y="4800599"/>
-          <a:ext cx="3248025" cy="857251"/>
+          <a:off x="8287803" y="1063626"/>
+          <a:ext cx="2888191" cy="904876"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -2415,18 +3092,262 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="ctr"/>
-          <a:fld id="{52D6CB36-8EA5-4E73-BBE0-2A585CF0AFAC}" type="TxLink">
-            <a:rPr lang="pt-BR" sz="6000"/>
-            <a:pPr algn="ctr"/>
-            <a:t>1350</a:t>
+          <a:fld id="{C0542029-D6B5-430F-B24B-DFC673FEF2D9}" type="TxLink">
+            <a:rPr lang="en-US" sz="3600" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="Aptos Narrow"/>
+            </a:rPr>
+            <a:t>R$ 940,00</a:t>
           </a:fld>
-          <a:endParaRPr lang="pt-BR" sz="6000"/>
+          <a:endParaRPr lang="pt-BR" sz="3600">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>279394</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>46567</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>596894</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>99484</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="CaixaDeTexto 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A62B202F-E12F-BF2E-94B5-6032534AF4F8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8015811" y="2015067"/>
+          <a:ext cx="3386666" cy="243417"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="accent5"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>TOTAL SUBSCRIPTIONS EA/PEASON PASS</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="1100" b="1">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>444497</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>158752</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>355047</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>58435</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Imagem 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0FF5E2B-1333-4205-A10D-70B402FB3C1A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6953247" y="1174752"/>
+          <a:ext cx="1138217" cy="852183"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>166687</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>142876</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>226218</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>107158</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="CaixaDeTexto 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{745F6B30-8FE3-0D09-7581-EA92B3EFD832}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4191000" y="2488407"/>
+          <a:ext cx="4917281" cy="345282"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="2000" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>TOTAL SUBSCRIPTIONS XBOX GAME PASS</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.25667</cdr:x>
+      <cdr:y>0.07014</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.78881</cdr:x>
+      <cdr:y>0.19571</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="CaixaDeTexto 2">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01CA9D17-D3AB-E238-02DC-C4F8E97C5121}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="2423454" y="246072"/>
+          <a:ext cx="5024437" cy="440531"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="pt-BR" sz="1100" kern="1200"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7209,7 +8130,373 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000001000000}" name="Tbl_anual_total" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0E910F21-28F6-4A07-A76E-8D08C51DEB0C}" name="Tabela dinâmica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+  <location ref="B31:C35" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="13">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="281">
+        <item x="87"/>
+        <item x="61"/>
+        <item x="206"/>
+        <item x="275"/>
+        <item x="112"/>
+        <item x="228"/>
+        <item x="35"/>
+        <item x="253"/>
+        <item x="136"/>
+        <item x="3"/>
+        <item x="161"/>
+        <item x="185"/>
+        <item x="7"/>
+        <item x="88"/>
+        <item x="16"/>
+        <item x="186"/>
+        <item x="162"/>
+        <item x="276"/>
+        <item x="36"/>
+        <item x="254"/>
+        <item x="207"/>
+        <item x="137"/>
+        <item x="62"/>
+        <item x="9"/>
+        <item x="113"/>
+        <item x="229"/>
+        <item x="163"/>
+        <item x="15"/>
+        <item x="6"/>
+        <item x="63"/>
+        <item x="37"/>
+        <item x="230"/>
+        <item x="255"/>
+        <item x="277"/>
+        <item x="138"/>
+        <item x="89"/>
+        <item x="114"/>
+        <item x="17"/>
+        <item x="187"/>
+        <item x="90"/>
+        <item x="139"/>
+        <item x="18"/>
+        <item x="38"/>
+        <item x="64"/>
+        <item x="231"/>
+        <item x="208"/>
+        <item x="256"/>
+        <item x="278"/>
+        <item x="13"/>
+        <item x="115"/>
+        <item x="164"/>
+        <item x="91"/>
+        <item x="188"/>
+        <item x="19"/>
+        <item x="209"/>
+        <item x="116"/>
+        <item x="257"/>
+        <item x="279"/>
+        <item x="140"/>
+        <item x="65"/>
+        <item x="39"/>
+        <item x="92"/>
+        <item x="210"/>
+        <item x="141"/>
+        <item x="232"/>
+        <item x="258"/>
+        <item x="40"/>
+        <item x="66"/>
+        <item x="117"/>
+        <item x="5"/>
+        <item x="165"/>
+        <item x="14"/>
+        <item x="67"/>
+        <item x="211"/>
+        <item x="189"/>
+        <item x="259"/>
+        <item x="20"/>
+        <item x="93"/>
+        <item x="233"/>
+        <item x="41"/>
+        <item x="142"/>
+        <item x="166"/>
+        <item x="143"/>
+        <item x="94"/>
+        <item x="212"/>
+        <item x="167"/>
+        <item x="68"/>
+        <item x="42"/>
+        <item x="234"/>
+        <item x="118"/>
+        <item x="21"/>
+        <item x="260"/>
+        <item x="144"/>
+        <item x="190"/>
+        <item x="213"/>
+        <item x="168"/>
+        <item x="43"/>
+        <item x="235"/>
+        <item x="119"/>
+        <item x="95"/>
+        <item x="22"/>
+        <item x="69"/>
+        <item x="145"/>
+        <item x="191"/>
+        <item x="169"/>
+        <item x="120"/>
+        <item x="261"/>
+        <item x="96"/>
+        <item x="236"/>
+        <item x="0"/>
+        <item x="23"/>
+        <item x="44"/>
+        <item x="70"/>
+        <item x="71"/>
+        <item x="97"/>
+        <item x="170"/>
+        <item x="262"/>
+        <item x="237"/>
+        <item x="146"/>
+        <item x="45"/>
+        <item x="24"/>
+        <item x="121"/>
+        <item x="12"/>
+        <item x="2"/>
+        <item x="192"/>
+        <item x="72"/>
+        <item x="263"/>
+        <item x="171"/>
+        <item x="238"/>
+        <item x="46"/>
+        <item x="98"/>
+        <item x="214"/>
+        <item x="147"/>
+        <item x="193"/>
+        <item x="264"/>
+        <item x="99"/>
+        <item x="172"/>
+        <item x="47"/>
+        <item x="122"/>
+        <item x="11"/>
+        <item x="239"/>
+        <item x="148"/>
+        <item x="215"/>
+        <item x="1"/>
+        <item x="25"/>
+        <item x="73"/>
+        <item x="123"/>
+        <item x="216"/>
+        <item x="265"/>
+        <item x="149"/>
+        <item x="240"/>
+        <item x="194"/>
+        <item x="26"/>
+        <item x="48"/>
+        <item x="173"/>
+        <item x="100"/>
+        <item x="74"/>
+        <item x="195"/>
+        <item x="174"/>
+        <item x="124"/>
+        <item x="241"/>
+        <item x="266"/>
+        <item x="49"/>
+        <item x="101"/>
+        <item x="150"/>
+        <item x="217"/>
+        <item x="75"/>
+        <item x="27"/>
+        <item x="151"/>
+        <item x="102"/>
+        <item x="218"/>
+        <item x="242"/>
+        <item x="267"/>
+        <item x="125"/>
+        <item x="50"/>
+        <item x="28"/>
+        <item x="76"/>
+        <item x="196"/>
+        <item x="175"/>
+        <item x="4"/>
+        <item x="126"/>
+        <item x="219"/>
+        <item x="268"/>
+        <item x="77"/>
+        <item x="51"/>
+        <item x="152"/>
+        <item x="243"/>
+        <item x="127"/>
+        <item x="103"/>
+        <item x="244"/>
+        <item x="29"/>
+        <item x="197"/>
+        <item x="176"/>
+        <item x="78"/>
+        <item x="269"/>
+        <item x="52"/>
+        <item x="153"/>
+        <item x="10"/>
+        <item x="79"/>
+        <item x="104"/>
+        <item x="30"/>
+        <item x="177"/>
+        <item x="220"/>
+        <item x="245"/>
+        <item x="270"/>
+        <item x="128"/>
+        <item x="8"/>
+        <item x="154"/>
+        <item x="198"/>
+        <item x="53"/>
+        <item x="31"/>
+        <item x="271"/>
+        <item x="246"/>
+        <item x="105"/>
+        <item x="178"/>
+        <item x="221"/>
+        <item x="80"/>
+        <item x="129"/>
+        <item x="155"/>
+        <item x="54"/>
+        <item x="199"/>
+        <item x="247"/>
+        <item x="55"/>
+        <item x="106"/>
+        <item x="179"/>
+        <item x="81"/>
+        <item x="156"/>
+        <item x="222"/>
+        <item x="200"/>
+        <item x="130"/>
+        <item x="248"/>
+        <item x="56"/>
+        <item x="223"/>
+        <item x="157"/>
+        <item x="131"/>
+        <item x="180"/>
+        <item x="201"/>
+        <item x="82"/>
+        <item x="107"/>
+        <item x="32"/>
+        <item x="158"/>
+        <item x="132"/>
+        <item x="202"/>
+        <item x="83"/>
+        <item x="181"/>
+        <item x="224"/>
+        <item x="249"/>
+        <item x="57"/>
+        <item x="108"/>
+        <item x="203"/>
+        <item x="133"/>
+        <item x="225"/>
+        <item x="109"/>
+        <item x="272"/>
+        <item x="182"/>
+        <item x="84"/>
+        <item x="250"/>
+        <item x="58"/>
+        <item x="110"/>
+        <item x="59"/>
+        <item x="183"/>
+        <item x="226"/>
+        <item x="85"/>
+        <item x="273"/>
+        <item x="159"/>
+        <item x="33"/>
+        <item x="204"/>
+        <item x="251"/>
+        <item x="134"/>
+        <item x="205"/>
+        <item x="60"/>
+        <item x="184"/>
+        <item x="160"/>
+        <item x="274"/>
+        <item x="227"/>
+        <item x="135"/>
+        <item x="86"/>
+        <item x="34"/>
+        <item x="252"/>
+        <item x="111"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="44" showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item sd="0" x="0"/>
+        <item sd="0" x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="44" showAll="0"/>
+    <pivotField numFmtId="44" showAll="0"/>
+    <pivotField numFmtId="44" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="6" item="0" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Soma de Minecraft Season Pass Price" fld="10" baseField="0" baseItem="0" numFmtId="44"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000001000000}" name="Tbl_anual_total" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
   <location ref="B11:C14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
@@ -7541,16 +8828,40 @@
     <i/>
   </colItems>
   <pageFields count="1">
-    <pageField fld="6" item="1" hier="-1"/>
+    <pageField fld="6" item="0" hier="-1"/>
   </pageFields>
   <dataFields count="1">
     <dataField name="Soma de Total Value" fld="12" baseField="1" baseItem="0" numFmtId="164"/>
   </dataFields>
-  <chartFormats count="1">
+  <chartFormats count="3">
     <chartFormat chart="2" format="2" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="3">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="4">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
             <x v="0"/>
           </reference>
         </references>
@@ -7569,7 +8880,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="Tbl_pass_total" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="B21:C25" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="13">
@@ -7918,7 +9229,7 @@
     <i/>
   </colItems>
   <pageFields count="1">
-    <pageField fld="6" item="1" hier="-1"/>
+    <pageField fld="6" item="0" hier="-1"/>
   </pageFields>
   <dataFields count="1">
     <dataField name="Soma de EA Play Season Pass" fld="8" baseField="2" baseItem="0"/>
@@ -7940,12 +9251,13 @@
   <pivotTables>
     <pivotTable tabId="6" name="Tbl_anual_total"/>
     <pivotTable tabId="6" name="Tbl_pass_total"/>
+    <pivotTable tabId="6" name="Tabela dinâmica1"/>
   </pivotTables>
   <data>
     <tabular pivotCacheId="1">
       <items count="3">
-        <i x="1"/>
-        <i x="0" s="1"/>
+        <i x="1" s="1"/>
+        <i x="0"/>
         <i x="2"/>
       </items>
     </tabular>
@@ -7955,12 +9267,12 @@
 
 <file path=xl/slicers/slicer1.xml><?xml version="1.0" encoding="utf-8"?>
 <slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10">
-  <slicer name="Subscription Type" xr10:uid="{00000000-0014-0000-FFFF-FFFF01000000}" cache="SegmentaçãodeDados_Subscription_Type" caption="Subscription Type" style="SlicerStyleDark6" rowHeight="241300"/>
+  <slicer name="Subscription Type" xr10:uid="{00000000-0014-0000-FFFF-FFFF01000000}" cache="SegmentaçãodeDados_Subscription_Type" caption="Subscription Type" style="Estilo de Segmentação de Dados 3" rowHeight="241300"/>
 </slicers>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="tbl_anual_total" displayName="tbl_anual_total" ref="A1:M296" totalsRowShown="0" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="tbl_anual_total" displayName="tbl_anual_total" ref="A1:M296" totalsRowShown="0" dataDxfId="15">
   <autoFilter ref="A1:M296" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="7">
       <filters>
@@ -7969,19 +9281,19 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Subscriber ID" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Plan" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Start Date" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Auto Renewal" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Subscription Price" dataDxfId="7" dataCellStyle="Moeda"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Subscription Type" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="EA Play Season Pass" dataDxfId="5"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="EA Play Season Pass_x000a_Price" dataDxfId="4" dataCellStyle="Moeda"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Minecraft Season Pass" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Minecraft Season Pass Price" dataDxfId="2" dataCellStyle="Moeda"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Coupon Value" dataDxfId="1" dataCellStyle="Moeda"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Total Value" dataDxfId="0" dataCellStyle="Moeda"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Subscriber ID" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Plan" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Start Date" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Auto Renewal" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Subscription Price" dataDxfId="9" dataCellStyle="Moeda"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Subscription Type" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="EA Play Season Pass" dataDxfId="7"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="EA Play Season Pass_x000a_Price" dataDxfId="6" dataCellStyle="Moeda"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Minecraft Season Pass" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Minecraft Season Pass Price" dataDxfId="4" dataCellStyle="Moeda"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Coupon Value" dataDxfId="3" dataCellStyle="Moeda"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Total Value" dataDxfId="2" dataCellStyle="Moeda"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8309,8 +9621,8 @@
   </sheetPr>
   <dimension ref="B3:N36"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView showGridLines="0" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8368,6 +9680,7 @@
       <c r="D22" s="14"/>
       <c r="E22" s="14"/>
       <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23" s="14"/>
@@ -8375,6 +9688,7 @@
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
       <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B24" s="14"/>
@@ -8382,6 +9696,7 @@
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
       <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B25" s="14"/>
@@ -8389,6 +9704,7 @@
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
       <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B26" s="14"/>
@@ -8396,6 +9712,7 @@
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
       <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B27" s="14"/>
@@ -8403,6 +9720,7 @@
       <c r="D27" s="14"/>
       <c r="E27" s="14"/>
       <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B28" s="14"/>
@@ -8410,6 +9728,7 @@
       <c r="D28" s="14"/>
       <c r="E28" s="14"/>
       <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B29" s="14"/>
@@ -8417,6 +9736,7 @@
       <c r="D29" s="14"/>
       <c r="E29" s="14"/>
       <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B30" s="14"/>
@@ -8424,6 +9744,7 @@
       <c r="D30" s="14"/>
       <c r="E30" s="14"/>
       <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B31" s="14"/>
@@ -8431,6 +9752,7 @@
       <c r="D31" s="14"/>
       <c r="E31" s="14"/>
       <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B32" s="14"/>
@@ -8438,34 +9760,39 @@
       <c r="D32" s="14"/>
       <c r="E32" s="14"/>
       <c r="F32" s="14"/>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G32" s="14"/>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="14"/>
       <c r="C33" s="14"/>
       <c r="D33" s="14"/>
       <c r="E33" s="14"/>
       <c r="F33" s="14"/>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G33" s="14"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="14"/>
       <c r="C34" s="14"/>
       <c r="D34" s="14"/>
       <c r="E34" s="14"/>
       <c r="F34" s="14"/>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G34" s="14"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="14"/>
       <c r="C35" s="14"/>
       <c r="D35" s="14"/>
       <c r="E35" s="14"/>
       <c r="F35" s="14"/>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G35" s="14"/>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="14"/>
       <c r="C36" s="14"/>
       <c r="D36" s="14"/>
       <c r="E36" s="14"/>
       <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -20652,17 +21979,18 @@
   <sheetPr>
     <tabColor theme="2" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="B3:I25"/>
+  <dimension ref="B3:I35"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
@@ -20692,7 +22020,7 @@
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
@@ -20708,7 +22036,7 @@
         <v>16</v>
       </c>
       <c r="C12" s="12">
-        <v>2824</v>
+        <v>217</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
@@ -20716,7 +22044,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="12">
-        <v>747</v>
+        <v>1537</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
@@ -20724,7 +22052,7 @@
         <v>311</v>
       </c>
       <c r="C14" s="12">
-        <v>3571</v>
+        <v>1754</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
@@ -20737,7 +22065,7 @@
         <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
@@ -20747,11 +22075,6 @@
       <c r="C21" t="s">
         <v>317</v>
       </c>
-      <c r="E21">
-        <f>GETPIVOTDATA("EA Play Season Pass
-Price",$B$21,"Plan","Ultimate")</f>
-        <v>1350</v>
-      </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="11" t="s">
@@ -20774,7 +22097,7 @@
         <v>11</v>
       </c>
       <c r="C24" s="18">
-        <v>1350</v>
+        <v>600</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
@@ -20782,7 +22105,69 @@
         <v>311</v>
       </c>
       <c r="C25" s="18">
-        <v>1350</v>
+        <v>600</v>
+      </c>
+      <c r="E25" s="20">
+        <f>GETPIVOTDATA("EA Play Season Pass
+Price",$B$21,"Plan","Ultimate")</f>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="10" t="s">
+        <v>310</v>
+      </c>
+      <c r="C31" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" s="19">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="19">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="11" t="s">
+        <v>311</v>
+      </c>
+      <c r="C35" s="19">
+        <v>940</v>
+      </c>
+      <c r="E35" s="20">
+        <f>GETPIVOTDATA("Minecraft Season Pass Price",$B$31)</f>
+        <v>940</v>
       </c>
     </row>
   </sheetData>
@@ -20800,8 +22185,8 @@
   </sheetPr>
   <dimension ref="A1:L94"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>